<commit_message>
7-th commit add to Cart funksiyasi hazirlandi Cart-daki masinlarin sayinin artirilmasi ile birge
</commit_message>
<xml_diff>
--- a/rentCar tree.xlsx
+++ b/rentCar tree.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aga77\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aga77\Desktop\rentCar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74782DC3-9C1C-4B02-A5B7-4AAF482B62CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E9F602-0F47-463B-B41E-6ECF43C9661F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{91781175-B0B7-4CC3-AC2A-D1F52E8E371F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>APP</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Cars</t>
+  </si>
+  <si>
+    <t>Cart</t>
   </si>
 </sst>
 </file>
@@ -74,7 +77,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -183,30 +186,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -215,6 +229,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -531,110 +564,140 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17C55EA-A3ED-41CB-9B7E-5F43E4F0897F}">
-  <dimension ref="I1:W8"/>
+  <dimension ref="I1:Z9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="V9" sqref="V9:W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="40" width="3.7109375" customWidth="1"/>
+    <col min="1" max="43" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="Q1" s="3" t="s">
+    <row r="1" spans="9:26" x14ac:dyDescent="0.3">
+      <c r="Q1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-    </row>
-    <row r="2" spans="9:23" x14ac:dyDescent="0.3">
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+    </row>
+    <row r="2" spans="9:26" x14ac:dyDescent="0.3">
       <c r="Q2" s="1"/>
-      <c r="W2" s="2"/>
-    </row>
-    <row r="3" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="Q3" s="3" t="s">
+      <c r="Z2" s="2"/>
+    </row>
+    <row r="3" spans="9:26" x14ac:dyDescent="0.3">
+      <c r="Q3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="R3" s="3"/>
-      <c r="V3" s="3" t="s">
+      <c r="R3" s="14"/>
+      <c r="Y3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="W3" s="3"/>
-    </row>
-    <row r="4" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="P4" s="8"/>
+      <c r="Z3" s="14"/>
+    </row>
+    <row r="4" spans="9:26" x14ac:dyDescent="0.3">
+      <c r="Q4" s="15"/>
+      <c r="R4" s="3"/>
       <c r="S4" s="9"/>
-      <c r="W4" s="2"/>
-    </row>
-    <row r="5" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="O5" s="3" t="s">
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="16"/>
+    </row>
+    <row r="5" spans="9:26" x14ac:dyDescent="0.3">
+      <c r="P5" s="5"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="6"/>
+      <c r="W5" s="4"/>
+      <c r="Z5" s="2"/>
+    </row>
+    <row r="6" spans="9:26" x14ac:dyDescent="0.3">
+      <c r="O6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="10"/>
-      <c r="S5" s="3" t="s">
+      <c r="P6" s="14"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="T5" s="3"/>
-      <c r="V5" s="3" t="s">
+      <c r="S6" s="14"/>
+      <c r="V6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="W6" s="14"/>
+      <c r="Y6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="W5" s="3"/>
-    </row>
-    <row r="6" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="10"/>
-    </row>
-    <row r="7" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="J7" s="8"/>
-      <c r="M7" s="11"/>
+      <c r="Z6" s="14"/>
+    </row>
+    <row r="7" spans="9:26" x14ac:dyDescent="0.3">
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="9"/>
       <c r="S7" s="7"/>
-    </row>
-    <row r="8" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="I8" s="4" t="s">
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="18"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
+    </row>
+    <row r="8" spans="9:26" x14ac:dyDescent="0.3">
+      <c r="J8" s="5"/>
+      <c r="M8" s="8"/>
+      <c r="S8" s="4"/>
+      <c r="W8" s="4"/>
+    </row>
+    <row r="9" spans="9:26" x14ac:dyDescent="0.3">
+      <c r="I9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="6"/>
-      <c r="L8" s="4" t="s">
+      <c r="J9" s="13"/>
+      <c r="L9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="6"/>
-      <c r="Q8" s="3" t="s">
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="13"/>
+      <c r="Q9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="W9" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="L8:O8"/>
-    <mergeCell ref="I8:J8"/>
+  <mergeCells count="11">
+    <mergeCell ref="L9:O9"/>
+    <mergeCell ref="I9:J9"/>
     <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="Q1:W1"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="Q8:T8"/>
-    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="Q9:T9"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="V9:W9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>